<commit_message>
Added listener and created html report
</commit_message>
<xml_diff>
--- a/src/main/java/bw_testData/loginDetails.xlsx
+++ b/src/main/java/bw_testData/loginDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Kiosk SDET\Application Interface &amp; E2E QA\bookswagon\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quality Kiosk SDET\Application Interface &amp; E2E QA\bookswagon\src\main\java\bw_testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBE69DF-45EF-4EBA-B64F-5937515BF229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7196C27-E060-4B36-BA95-6A67142085D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{414E33EA-1472-4827-90ED-D736CFE0909B}"/>
+    <workbookView xWindow="12972" yWindow="1572" windowWidth="7608" windowHeight="9612" xr2:uid="{414E33EA-1472-4827-90ED-D736CFE0909B}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>ghi</t>
+  </si>
+  <si>
+    <t>prakash@gmail.com</t>
+  </si>
+  <si>
+    <t>prakassh</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EFABAD-80B8-4C79-BBCF-95AABE5716FA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,11 +469,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E4C30C4C-1540-4B82-8D50-1EA260156663}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{07ECC5C0-C596-4FAC-8606-17150A65A20A}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{41A83D4E-2DAF-46CF-81DE-D361AE0845B9}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F3C6A328-DC4B-42E2-9DF2-B0FAE780A101}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>